<commit_message>
Updated database table lists
</commit_message>
<xml_diff>
--- a/Documentations/数据分析表格汇总.xlsx
+++ b/Documentations/数据分析表格汇总.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alan\Documents\GitHub\jiaanpei\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alan\Documents\GitHub\jiaanpei\Documentations\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="154">
   <si>
     <t>表名</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -583,6 +583,54 @@
   </si>
   <si>
     <t>车享配数据与杭州本地化价格对比分析</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>youshanding</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>import</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>基础</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>优闪订基础供货数据</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>无</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>youshanding_zhejiang_local_cmp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>analysis</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>分析</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>优闪订数据与浙江本地化价格对比分析</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>youshanding_zhejiang_cmp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>zhejiang_local</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>youshanding</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1018,10 +1066,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H40"/>
+  <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40:H40"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1906,26 +1954,26 @@
         <v>42915</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A37" t="s">
+    <row r="37" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A37" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B37" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C37" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="D37" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="E37" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="G37" s="1" t="s">
+      <c r="E37" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="G37" s="4" t="s">
         <v>81</v>
       </c>
     </row>
@@ -2005,6 +2053,58 @@
       </c>
       <c r="H40" s="3">
         <v>42945</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A41" t="s">
+        <v>142</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="H41" s="3">
+        <v>42949</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="A42" t="s">
+        <v>147</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="H42" s="3">
+        <v>42949</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated database table list
</commit_message>
<xml_diff>
--- a/Documentations/数据分析表格汇总.xlsx
+++ b/Documentations/数据分析表格汇总.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="158">
   <si>
     <t>表名</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -631,6 +631,22 @@
   </si>
   <si>
     <t>youshanding</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>youshanding_hangzhou_claim_cmp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>分析</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>优闪订数据与杭州本地化价格对比分析</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>youshanding_hangzhou_cmp</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1066,10 +1082,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H42"/>
+  <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="J42" sqref="J42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2104,6 +2120,32 @@
         <v>153</v>
       </c>
       <c r="H42" s="3">
+        <v>42949</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="A43" t="s">
+        <v>154</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="H43" s="3">
         <v>42949</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated database tables list
</commit_message>
<xml_diff>
--- a/Documentations/数据分析表格汇总.xlsx
+++ b/Documentations/数据分析表格汇总.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="169">
   <si>
     <t>表名</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -647,6 +647,50 @@
   </si>
   <si>
     <t>youshanding_hangzhou_cmp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>guangzhouyihong</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>基础</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>广州一弘基础供货数据</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>无</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>无</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>guangzhouyihong_sichuan_claim_cmp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>analysis</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>分析</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>广州一弘数据与四川理赔数据对比分析</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>guangzhouyihong_cmp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>base_lclaim</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1082,10 +1126,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H43"/>
+  <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="J42" sqref="J42"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="H46" sqref="H46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2147,6 +2191,58 @@
       </c>
       <c r="H43" s="3">
         <v>42949</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A44" t="s">
+        <v>158</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="H44" s="3">
+        <v>42950</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="A45" t="s">
+        <v>163</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="H45" s="3">
+        <v>42950</v>
       </c>
     </row>
   </sheetData>

</xml_diff>